<commit_message>
modify UI/ socket server add init
</commit_message>
<xml_diff>
--- a/Socket電文規格v1.0.xlsx
+++ b/Socket電文規格v1.0.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="986" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="986"/>
   </bookViews>
   <sheets>
     <sheet name="訊息格式說明" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="56">
   <si>
     <t>Standard Header</t>
   </si>
@@ -701,6 +701,10 @@
       </rPr>
       <t>尚未開始檢測</t>
     </r>
+    <phoneticPr fontId="28" type="noConversion"/>
+  </si>
+  <si>
+    <t>預設port: 35010</t>
     <phoneticPr fontId="28" type="noConversion"/>
   </si>
 </sst>
@@ -1596,6 +1600,18 @@
     <xf numFmtId="0" fontId="30" fillId="0" borderId="10" xfId="20" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" xfId="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="31" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1631,18 +1647,6 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" xfId="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -2112,13 +2116,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:I32"/>
+  <dimension ref="B1:I34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="4.5" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="0.75" style="1" customWidth="1"/>
+    <col min="1" max="1" width="0.625" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.625" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.875" style="1" customWidth="1"/>
     <col min="4" max="4" width="8.5" style="1" bestFit="1" customWidth="1"/>
@@ -2130,244 +2136,241 @@
     <col min="10" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="4.5" customHeight="1" thickBot="1"/>
-    <row r="2" spans="2:9" ht="12.75" customHeight="1">
-      <c r="B2" s="55" t="s">
+    <row r="1" spans="2:9" ht="14.25"/>
+    <row r="2" spans="2:9" ht="14.25">
+      <c r="B2" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" ht="15" thickBot="1"/>
+    <row r="4" spans="2:9" ht="12.75" customHeight="1">
+      <c r="B4" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="58"/>
-    </row>
-    <row r="3" spans="2:9" ht="49.5" customHeight="1">
-      <c r="B3" s="51" t="s">
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="62"/>
+    </row>
+    <row r="5" spans="2:9" ht="49.5" customHeight="1">
+      <c r="B5" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="54"/>
-    </row>
-    <row r="4" spans="2:9" ht="12.75" customHeight="1">
-      <c r="B4" s="49" t="s">
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="57"/>
+      <c r="I5" s="58"/>
+    </row>
+    <row r="6" spans="2:9" ht="12.75" customHeight="1">
+      <c r="B6" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C6" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D6" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="E6" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F6" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="25" t="s">
+      <c r="G6" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="25" t="s">
+      <c r="H6" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="I4" s="26" t="s">
+      <c r="I6" s="26" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="14.25">
-      <c r="B5" s="50"/>
-      <c r="C5" s="27" t="s">
+    <row r="7" spans="2:9" ht="14.25">
+      <c r="B7" s="54"/>
+      <c r="C7" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="28">
+      <c r="D7" s="28">
         <v>0</v>
       </c>
-      <c r="E5" s="28">
-        <f>D5+F5-1</f>
+      <c r="E7" s="28">
+        <f>D7+F7-1</f>
         <v>3</v>
       </c>
-      <c r="F5" s="28">
+      <c r="F7" s="28">
         <v>4</v>
       </c>
-      <c r="G5" s="28" t="s">
+      <c r="G7" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="29"/>
-      <c r="I5" s="21" t="s">
+      <c r="H7" s="29"/>
+      <c r="I7" s="21" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="2:9" ht="14.25">
-      <c r="B6" s="50"/>
-      <c r="C6" s="27" t="s">
+    <row r="8" spans="2:9" ht="14.25">
+      <c r="B8" s="54"/>
+      <c r="C8" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="28">
-        <f>E5+1</f>
+      <c r="D8" s="28">
+        <f>E7+1</f>
         <v>4</v>
       </c>
-      <c r="E6" s="28">
-        <f>D6+F6-1</f>
+      <c r="E8" s="28">
+        <f>D8+F8-1</f>
         <v>5</v>
       </c>
-      <c r="F6" s="28">
+      <c r="F8" s="28">
         <v>2</v>
       </c>
-      <c r="G6" s="28" t="s">
+      <c r="G8" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="29"/>
-      <c r="I6" s="21" t="s">
+      <c r="H8" s="29"/>
+      <c r="I8" s="21" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="14.25">
-      <c r="B7" s="50"/>
-      <c r="C7" s="27" t="s">
+    <row r="9" spans="2:9" ht="14.25">
+      <c r="B9" s="54"/>
+      <c r="C9" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="28">
-        <f>E6+1</f>
+      <c r="D9" s="28">
+        <f>E8+1</f>
         <v>6</v>
       </c>
-      <c r="E7" s="28">
-        <f t="shared" ref="E7:E9" si="0">D7+F7-1</f>
+      <c r="E9" s="28">
+        <f t="shared" ref="E9:E11" si="0">D9+F9-1</f>
         <v>7</v>
       </c>
-      <c r="F7" s="30">
+      <c r="F9" s="30">
         <v>2</v>
       </c>
-      <c r="G7" s="28" t="s">
+      <c r="G9" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="31"/>
-      <c r="I7" s="21"/>
-    </row>
-    <row r="8" spans="2:9" ht="14.25">
-      <c r="B8" s="50"/>
-      <c r="C8" s="27" t="s">
+      <c r="H9" s="31"/>
+      <c r="I9" s="21"/>
+    </row>
+    <row r="10" spans="2:9" ht="14.25">
+      <c r="B10" s="54"/>
+      <c r="C10" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="28">
-        <f t="shared" ref="D8:D10" si="1">E7+1</f>
+      <c r="D10" s="28">
+        <f t="shared" ref="D10:D12" si="1">E9+1</f>
         <v>8</v>
       </c>
-      <c r="E8" s="28">
+      <c r="E10" s="28">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="F8" s="28">
+      <c r="F10" s="28">
         <v>1</v>
       </c>
-      <c r="G8" s="28" t="s">
+      <c r="G10" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="29"/>
-      <c r="I8" s="22"/>
-    </row>
-    <row r="9" spans="2:9" ht="14.25">
-      <c r="B9" s="50"/>
-      <c r="C9" s="28" t="s">
+      <c r="H10" s="29"/>
+      <c r="I10" s="22"/>
+    </row>
+    <row r="11" spans="2:9" ht="14.25">
+      <c r="B11" s="54"/>
+      <c r="C11" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="28">
-        <f>E8+1</f>
+      <c r="D11" s="28">
+        <f>E10+1</f>
         <v>9</v>
       </c>
-      <c r="E9" s="28">
+      <c r="E11" s="28">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="F9" s="28">
+      <c r="F11" s="28">
         <v>4</v>
       </c>
-      <c r="G9" s="28" t="s">
+      <c r="G11" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="28"/>
-      <c r="I9" s="22" t="s">
+      <c r="H11" s="28"/>
+      <c r="I11" s="22" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="2:9" ht="14.25">
-      <c r="B10" s="32" t="s">
+    <row r="12" spans="2:9" ht="14.25">
+      <c r="B12" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="33" t="s">
+      <c r="C12" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="28">
+      <c r="D12" s="28">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="E10" s="34" t="s">
+      <c r="E12" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="F10" s="34" t="s">
+      <c r="F12" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="23" t="s">
+      <c r="G12" s="33"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="23" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="2:9" ht="15" thickBot="1">
-      <c r="B11" s="35" t="s">
+    <row r="13" spans="2:9" ht="15" thickBot="1">
+      <c r="B13" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="C13" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D13" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="E11" s="19" t="s">
+      <c r="E13" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="20">
+      <c r="F13" s="20">
         <v>1</v>
       </c>
-      <c r="G11" s="37" t="s">
+      <c r="G13" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="20"/>
-      <c r="I11" s="24" t="s">
+      <c r="H13" s="20"/>
+      <c r="I13" s="24" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="2:9" ht="12.75" customHeight="1">
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="2:9" ht="12.75" customHeight="1"/>
-    <row r="14" spans="2:9" ht="16.5" customHeight="1">
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-    </row>
-    <row r="15" spans="2:9" ht="12.75" customHeight="1">
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-    </row>
-    <row r="16" spans="2:9" ht="12.75" customHeight="1">
-      <c r="B16" s="5"/>
-      <c r="C16" s="6"/>
+    <row r="14" spans="2:9" ht="12.75" customHeight="1">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+    </row>
+    <row r="15" spans="2:9" ht="12.75" customHeight="1"/>
+    <row r="16" spans="2:9" ht="16.5" customHeight="1">
+      <c r="C16" s="3"/>
     </row>
     <row r="17" spans="2:3" ht="12.75" customHeight="1">
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
     </row>
     <row r="18" spans="2:3" ht="12.75" customHeight="1">
-      <c r="B18" s="6"/>
+      <c r="B18" s="5"/>
       <c r="C18" s="6"/>
     </row>
     <row r="19" spans="2:3" ht="12.75" customHeight="1">
@@ -2376,59 +2379,67 @@
     </row>
     <row r="20" spans="2:3" ht="12.75" customHeight="1">
       <c r="B20" s="6"/>
-      <c r="C20" s="7"/>
+      <c r="C20" s="6"/>
     </row>
     <row r="21" spans="2:3" ht="12.75" customHeight="1">
       <c r="B21" s="6"/>
-      <c r="C21" s="7"/>
+      <c r="C21" s="6"/>
     </row>
     <row r="22" spans="2:3" ht="12.75" customHeight="1">
-      <c r="B22" s="7"/>
+      <c r="B22" s="6"/>
       <c r="C22" s="7"/>
     </row>
-    <row r="23" spans="2:3" ht="12.75" customHeight="1"/>
-    <row r="24" spans="2:3" ht="16.5" customHeight="1">
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-    </row>
-    <row r="25" spans="2:3" ht="12.75" customHeight="1">
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-    </row>
-    <row r="26" spans="2:3" ht="12.75" customHeight="1">
-      <c r="B26" s="5"/>
-      <c r="C26" s="6"/>
+    <row r="23" spans="2:3" ht="12.75" customHeight="1">
+      <c r="B23" s="6"/>
+      <c r="C23" s="7"/>
+    </row>
+    <row r="24" spans="2:3" ht="12.75" customHeight="1">
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+    </row>
+    <row r="25" spans="2:3" ht="12.75" customHeight="1"/>
+    <row r="26" spans="2:3" ht="16.5" customHeight="1">
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
     </row>
     <row r="27" spans="2:3" ht="12.75" customHeight="1">
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
     </row>
     <row r="28" spans="2:3" ht="12.75" customHeight="1">
-      <c r="B28" s="6"/>
+      <c r="B28" s="5"/>
       <c r="C28" s="6"/>
     </row>
     <row r="29" spans="2:3" ht="12.75" customHeight="1">
       <c r="B29" s="6"/>
-      <c r="C29" s="7"/>
+      <c r="C29" s="6"/>
     </row>
     <row r="30" spans="2:3" ht="12.75" customHeight="1">
       <c r="B30" s="6"/>
-      <c r="C30" s="7"/>
+      <c r="C30" s="6"/>
     </row>
     <row r="31" spans="2:3" ht="12.75" customHeight="1">
       <c r="B31" s="6"/>
       <c r="C31" s="7"/>
     </row>
     <row r="32" spans="2:3" ht="12.75" customHeight="1">
-      <c r="B32" s="7"/>
+      <c r="B32" s="6"/>
       <c r="C32" s="7"/>
+    </row>
+    <row r="33" spans="2:3" ht="12.75" customHeight="1">
+      <c r="B33" s="6"/>
+      <c r="C33" s="7"/>
+    </row>
+    <row r="34" spans="2:3" ht="12.75" customHeight="1">
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="3">
-    <mergeCell ref="B4:B9"/>
-    <mergeCell ref="B3:I3"/>
-    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B6:B11"/>
+    <mergeCell ref="B5:I5"/>
+    <mergeCell ref="B4:I4"/>
   </mergeCells>
   <phoneticPr fontId="28" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="0.97986111111111107" bottom="0.97986111111111107" header="0.51180555555555551" footer="0.51180555555555551"/>
@@ -2464,10 +2475,10 @@
       <c r="A3" s="42">
         <v>1</v>
       </c>
-      <c r="B3" s="63" t="s">
+      <c r="B3" s="51" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="64" t="s">
+      <c r="C3" s="52" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2475,7 +2486,7 @@
       <c r="A4" s="42">
         <v>2</v>
       </c>
-      <c r="B4" s="61" t="s">
+      <c r="B4" s="49" t="s">
         <v>48</v>
       </c>
       <c r="C4" s="42" t="s">
@@ -2486,7 +2497,7 @@
       <c r="A5" s="42">
         <v>3</v>
       </c>
-      <c r="B5" s="61" t="s">
+      <c r="B5" s="49" t="s">
         <v>51</v>
       </c>
       <c r="C5" s="42" t="s">
@@ -2525,17 +2536,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="12.75" customHeight="1">
-      <c r="B2" s="59" t="s">
+      <c r="B2" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="62" t="s">
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="50" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2544,31 +2555,31 @@
         <v>36</v>
       </c>
       <c r="C3" s="41" t="str">
-        <f>訊息格式說明!C4</f>
+        <f>訊息格式說明!C6</f>
         <v>欄位名稱</v>
       </c>
       <c r="D3" s="41" t="str">
-        <f>訊息格式說明!D4</f>
+        <f>訊息格式說明!D6</f>
         <v>起始位置</v>
       </c>
       <c r="E3" s="41" t="str">
-        <f>訊息格式說明!E4</f>
+        <f>訊息格式說明!E6</f>
         <v>結束位置</v>
       </c>
       <c r="F3" s="41" t="str">
-        <f>訊息格式說明!F4</f>
+        <f>訊息格式說明!F6</f>
         <v>欄位長度(byte)</v>
       </c>
       <c r="G3" s="41" t="str">
-        <f>訊息格式說明!G4</f>
+        <f>訊息格式說明!G6</f>
         <v>欄位型態(C#)</v>
       </c>
       <c r="H3" s="41" t="str">
-        <f>訊息格式說明!H4</f>
+        <f>訊息格式說明!H6</f>
         <v>非必填</v>
       </c>
       <c r="I3" s="41" t="str">
-        <f>訊息格式說明!I4</f>
+        <f>訊息格式說明!I6</f>
         <v>說明</v>
       </c>
     </row>
@@ -2577,28 +2588,28 @@
         <v>1</v>
       </c>
       <c r="C4" s="43" t="str">
-        <f>訊息格式說明!C5</f>
+        <f>訊息格式說明!C7</f>
         <v>起始字串</v>
       </c>
       <c r="D4" s="39">
-        <f>訊息格式說明!D5</f>
+        <f>訊息格式說明!D7</f>
         <v>0</v>
       </c>
       <c r="E4" s="39">
-        <f>訊息格式說明!E5</f>
+        <f>訊息格式說明!E7</f>
         <v>3</v>
       </c>
       <c r="F4" s="39">
-        <f>訊息格式說明!F5</f>
+        <f>訊息格式說明!F7</f>
         <v>4</v>
       </c>
       <c r="G4" s="39" t="str">
-        <f>訊息格式說明!G5</f>
+        <f>訊息格式說明!G7</f>
         <v>uint</v>
       </c>
       <c r="H4" s="44"/>
       <c r="I4" s="45" t="str">
-        <f>訊息格式說明!I5</f>
+        <f>訊息格式說明!I7</f>
         <v>0x494f41  (AOI)</v>
       </c>
     </row>
@@ -2607,28 +2618,28 @@
         <v>2</v>
       </c>
       <c r="C5" s="43" t="str">
-        <f>訊息格式說明!C6</f>
+        <f>訊息格式說明!C8</f>
         <v>版本</v>
       </c>
       <c r="D5" s="39">
-        <f>訊息格式說明!D6</f>
+        <f>訊息格式說明!D8</f>
         <v>4</v>
       </c>
       <c r="E5" s="39">
-        <f>訊息格式說明!E6</f>
+        <f>訊息格式說明!E8</f>
         <v>5</v>
       </c>
       <c r="F5" s="39">
-        <f>訊息格式說明!F6</f>
+        <f>訊息格式說明!F8</f>
         <v>2</v>
       </c>
       <c r="G5" s="39" t="str">
-        <f>訊息格式說明!G6</f>
+        <f>訊息格式說明!G8</f>
         <v>ushort</v>
       </c>
       <c r="H5" s="44"/>
       <c r="I5" s="45" t="str">
-        <f>訊息格式說明!I6</f>
+        <f>訊息格式說明!I8</f>
         <v>0x0100      (1.0)</v>
       </c>
     </row>
@@ -2637,23 +2648,23 @@
         <v>3</v>
       </c>
       <c r="C6" s="43" t="str">
-        <f>訊息格式說明!C7</f>
+        <f>訊息格式說明!C9</f>
         <v>保留欄位</v>
       </c>
       <c r="D6" s="39">
-        <f>訊息格式說明!D7</f>
+        <f>訊息格式說明!D9</f>
         <v>6</v>
       </c>
       <c r="E6" s="39">
-        <f>訊息格式說明!E7</f>
+        <f>訊息格式說明!E9</f>
         <v>7</v>
       </c>
       <c r="F6" s="39">
-        <f>訊息格式說明!F7</f>
+        <f>訊息格式說明!F9</f>
         <v>2</v>
       </c>
       <c r="G6" s="39" t="str">
-        <f>訊息格式說明!G7</f>
+        <f>訊息格式說明!G9</f>
         <v>ushort</v>
       </c>
       <c r="H6" s="46"/>
@@ -2665,23 +2676,23 @@
         <v>4</v>
       </c>
       <c r="C7" s="43" t="str">
-        <f>訊息格式說明!C8</f>
+        <f>訊息格式說明!C10</f>
         <v>訊息種類</v>
       </c>
       <c r="D7" s="39">
-        <f>訊息格式說明!D8</f>
+        <f>訊息格式說明!D10</f>
         <v>8</v>
       </c>
       <c r="E7" s="39">
-        <f>訊息格式說明!E8</f>
+        <f>訊息格式說明!E10</f>
         <v>8</v>
       </c>
       <c r="F7" s="39">
-        <f>訊息格式說明!F8</f>
+        <f>訊息格式說明!F10</f>
         <v>1</v>
       </c>
       <c r="G7" s="39" t="str">
-        <f>訊息格式說明!G8</f>
+        <f>訊息格式說明!G10</f>
         <v>byte</v>
       </c>
       <c r="H7" s="44"/>
@@ -2694,23 +2705,23 @@
         <v>5</v>
       </c>
       <c r="C8" s="43" t="str">
-        <f>訊息格式說明!C9</f>
+        <f>訊息格式說明!C11</f>
         <v>body長度</v>
       </c>
       <c r="D8" s="39">
-        <f>訊息格式說明!D9</f>
+        <f>訊息格式說明!D11</f>
         <v>9</v>
       </c>
       <c r="E8" s="39">
-        <f>訊息格式說明!E9</f>
+        <f>訊息格式說明!E11</f>
         <v>12</v>
       </c>
       <c r="F8" s="39">
-        <f>訊息格式說明!F9</f>
+        <f>訊息格式說明!F11</f>
         <v>4</v>
       </c>
       <c r="G8" s="39" t="str">
-        <f>訊息格式說明!G9</f>
+        <f>訊息格式說明!G11</f>
         <v>int</v>
       </c>
       <c r="H8" s="39"/>
@@ -2749,7 +2760,7 @@
         <v>7</v>
       </c>
       <c r="C10" s="39" t="str">
-        <f>訊息格式說明!C11</f>
+        <f>訊息格式說明!C13</f>
         <v>CheckSum</v>
       </c>
       <c r="D10" s="39">
@@ -2761,16 +2772,16 @@
         <v>14</v>
       </c>
       <c r="F10" s="39">
-        <f>訊息格式說明!F11</f>
+        <f>訊息格式說明!F13</f>
         <v>1</v>
       </c>
       <c r="G10" s="39" t="str">
-        <f>訊息格式說明!G11</f>
+        <f>訊息格式說明!G13</f>
         <v>byte</v>
       </c>
       <c r="H10" s="39"/>
       <c r="I10" s="39" t="str">
-        <f>訊息格式說明!I11</f>
+        <f>訊息格式說明!I13</f>
         <v>除起始字串及CheckSum外的欄位以XOR做加總</v>
       </c>
     </row>
@@ -2795,7 +2806,7 @@
   <dimension ref="B1:J30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2813,17 +2824,17 @@
   <sheetData>
     <row r="1" spans="2:10" ht="5.25" customHeight="1"/>
     <row r="2" spans="2:10" ht="13.5" customHeight="1">
-      <c r="B2" s="60" t="s">
+      <c r="B2" s="64" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="62" t="s">
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="50" t="s">
         <v>2</v>
       </c>
     </row>
@@ -2832,31 +2843,31 @@
         <v>6</v>
       </c>
       <c r="C3" s="9" t="str">
-        <f>訊息格式說明!C4</f>
+        <f>訊息格式說明!C6</f>
         <v>欄位名稱</v>
       </c>
       <c r="D3" s="9" t="str">
-        <f>訊息格式說明!D4</f>
+        <f>訊息格式說明!D6</f>
         <v>起始位置</v>
       </c>
       <c r="E3" s="9" t="str">
-        <f>訊息格式說明!E4</f>
+        <f>訊息格式說明!E6</f>
         <v>結束位置</v>
       </c>
       <c r="F3" s="9" t="str">
-        <f>訊息格式說明!F4</f>
+        <f>訊息格式說明!F6</f>
         <v>欄位長度(byte)</v>
       </c>
       <c r="G3" s="9" t="str">
-        <f>訊息格式說明!G4</f>
+        <f>訊息格式說明!G6</f>
         <v>欄位型態(C#)</v>
       </c>
       <c r="H3" s="9" t="str">
-        <f>訊息格式說明!H4</f>
+        <f>訊息格式說明!H6</f>
         <v>非必填</v>
       </c>
       <c r="I3" s="9" t="str">
-        <f>訊息格式說明!I4</f>
+        <f>訊息格式說明!I6</f>
         <v>說明</v>
       </c>
     </row>
@@ -2865,28 +2876,28 @@
         <v>1</v>
       </c>
       <c r="C4" s="15" t="str">
-        <f>訊息格式說明!C5</f>
+        <f>訊息格式說明!C7</f>
         <v>起始字串</v>
       </c>
       <c r="D4" s="11">
-        <f>訊息格式說明!D5</f>
+        <f>訊息格式說明!D7</f>
         <v>0</v>
       </c>
       <c r="E4" s="11">
-        <f>訊息格式說明!E5</f>
+        <f>訊息格式說明!E7</f>
         <v>3</v>
       </c>
       <c r="F4" s="11">
-        <f>訊息格式說明!F5</f>
+        <f>訊息格式說明!F7</f>
         <v>4</v>
       </c>
       <c r="G4" s="11" t="str">
-        <f>訊息格式說明!G5</f>
+        <f>訊息格式說明!G7</f>
         <v>uint</v>
       </c>
       <c r="H4" s="16"/>
       <c r="I4" s="17" t="str">
-        <f>訊息格式說明!I5</f>
+        <f>訊息格式說明!I7</f>
         <v>0x494f41  (AOI)</v>
       </c>
     </row>
@@ -2895,28 +2906,28 @@
         <v>2</v>
       </c>
       <c r="C5" s="15" t="str">
-        <f>訊息格式說明!C6</f>
+        <f>訊息格式說明!C8</f>
         <v>版本</v>
       </c>
       <c r="D5" s="11">
-        <f>訊息格式說明!D6</f>
+        <f>訊息格式說明!D8</f>
         <v>4</v>
       </c>
       <c r="E5" s="11">
-        <f>訊息格式說明!E6</f>
+        <f>訊息格式說明!E8</f>
         <v>5</v>
       </c>
       <c r="F5" s="11">
-        <f>訊息格式說明!F6</f>
+        <f>訊息格式說明!F8</f>
         <v>2</v>
       </c>
       <c r="G5" s="11" t="str">
-        <f>訊息格式說明!G6</f>
+        <f>訊息格式說明!G8</f>
         <v>ushort</v>
       </c>
       <c r="H5" s="16"/>
       <c r="I5" s="17" t="str">
-        <f>訊息格式說明!I6</f>
+        <f>訊息格式說明!I8</f>
         <v>0x0100      (1.0)</v>
       </c>
     </row>
@@ -2925,23 +2936,23 @@
         <v>3</v>
       </c>
       <c r="C6" s="15" t="str">
-        <f>訊息格式說明!C7</f>
+        <f>訊息格式說明!C9</f>
         <v>保留欄位</v>
       </c>
       <c r="D6" s="11">
-        <f>訊息格式說明!D7</f>
+        <f>訊息格式說明!D9</f>
         <v>6</v>
       </c>
       <c r="E6" s="11">
-        <f>訊息格式說明!E7</f>
+        <f>訊息格式說明!E9</f>
         <v>7</v>
       </c>
       <c r="F6" s="11">
-        <f>訊息格式說明!F7</f>
+        <f>訊息格式說明!F9</f>
         <v>2</v>
       </c>
       <c r="G6" s="11" t="str">
-        <f>訊息格式說明!G7</f>
+        <f>訊息格式說明!G9</f>
         <v>ushort</v>
       </c>
       <c r="H6" s="18"/>
@@ -2952,23 +2963,23 @@
         <v>4</v>
       </c>
       <c r="C7" s="15" t="str">
-        <f>訊息格式說明!C8</f>
+        <f>訊息格式說明!C10</f>
         <v>訊息種類</v>
       </c>
       <c r="D7" s="11">
-        <f>訊息格式說明!D8</f>
+        <f>訊息格式說明!D10</f>
         <v>8</v>
       </c>
       <c r="E7" s="11">
-        <f>訊息格式說明!E8</f>
+        <f>訊息格式說明!E10</f>
         <v>8</v>
       </c>
       <c r="F7" s="11">
-        <f>訊息格式說明!F8</f>
+        <f>訊息格式說明!F10</f>
         <v>1</v>
       </c>
       <c r="G7" s="11" t="str">
-        <f>訊息格式說明!G8</f>
+        <f>訊息格式說明!G10</f>
         <v>byte</v>
       </c>
       <c r="H7" s="16"/>
@@ -2981,23 +2992,23 @@
         <v>5</v>
       </c>
       <c r="C8" s="15" t="str">
-        <f>訊息格式說明!C9</f>
+        <f>訊息格式說明!C11</f>
         <v>body長度</v>
       </c>
       <c r="D8" s="11">
-        <f>訊息格式說明!D9</f>
+        <f>訊息格式說明!D11</f>
         <v>9</v>
       </c>
       <c r="E8" s="11">
-        <f>訊息格式說明!E9</f>
+        <f>訊息格式說明!E11</f>
         <v>12</v>
       </c>
       <c r="F8" s="11">
-        <f>訊息格式說明!F9</f>
+        <f>訊息格式說明!F11</f>
         <v>4</v>
       </c>
       <c r="G8" s="11" t="str">
-        <f>訊息格式說明!G9</f>
+        <f>訊息格式說明!G11</f>
         <v>int</v>
       </c>
       <c r="H8" s="10"/>
@@ -3071,16 +3082,16 @@
         <v>18</v>
       </c>
       <c r="F11" s="11">
-        <f>訊息格式說明!F11</f>
+        <f>訊息格式說明!F13</f>
         <v>1</v>
       </c>
       <c r="G11" s="11" t="str">
-        <f>訊息格式說明!G11</f>
+        <f>訊息格式說明!G13</f>
         <v>byte</v>
       </c>
       <c r="H11" s="10"/>
       <c r="I11" s="10" t="str">
-        <f>訊息格式說明!I11</f>
+        <f>訊息格式說明!I13</f>
         <v>除起始字串及CheckSum外的欄位以XOR做加總</v>
       </c>
     </row>
@@ -3160,8 +3171,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -3173,50 +3184,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="64" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="62" t="s">
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="50" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" ht="27">
       <c r="A2" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="9" t="str">
-        <f>訊息格式說明!C4</f>
+        <f>訊息格式說明!C6</f>
         <v>欄位名稱</v>
       </c>
       <c r="C2" s="9" t="str">
-        <f>訊息格式說明!D4</f>
+        <f>訊息格式說明!D6</f>
         <v>起始位置</v>
       </c>
       <c r="D2" s="9" t="str">
-        <f>訊息格式說明!E4</f>
+        <f>訊息格式說明!E6</f>
         <v>結束位置</v>
       </c>
       <c r="E2" s="9" t="str">
-        <f>訊息格式說明!F4</f>
+        <f>訊息格式說明!F6</f>
         <v>欄位長度(byte)</v>
       </c>
       <c r="F2" s="9" t="str">
-        <f>訊息格式說明!G4</f>
+        <f>訊息格式說明!G6</f>
         <v>欄位型態(C#)</v>
       </c>
       <c r="G2" s="9" t="str">
-        <f>訊息格式說明!H4</f>
+        <f>訊息格式說明!H6</f>
         <v>非必填</v>
       </c>
       <c r="H2" s="9" t="str">
-        <f>訊息格式說明!I4</f>
+        <f>訊息格式說明!I6</f>
         <v>說明</v>
       </c>
       <c r="I2" s="1"/>
@@ -3226,28 +3237,28 @@
         <v>1</v>
       </c>
       <c r="B3" s="15" t="str">
-        <f>訊息格式說明!C5</f>
+        <f>訊息格式說明!C7</f>
         <v>起始字串</v>
       </c>
       <c r="C3" s="11">
-        <f>訊息格式說明!D5</f>
+        <f>訊息格式說明!D7</f>
         <v>0</v>
       </c>
       <c r="D3" s="11">
-        <f>訊息格式說明!E5</f>
+        <f>訊息格式說明!E7</f>
         <v>3</v>
       </c>
       <c r="E3" s="11">
-        <f>訊息格式說明!F5</f>
+        <f>訊息格式說明!F7</f>
         <v>4</v>
       </c>
       <c r="F3" s="11" t="str">
-        <f>訊息格式說明!G5</f>
+        <f>訊息格式說明!G7</f>
         <v>uint</v>
       </c>
       <c r="G3" s="16"/>
       <c r="H3" s="17" t="str">
-        <f>訊息格式說明!I5</f>
+        <f>訊息格式說明!I7</f>
         <v>0x494f41  (AOI)</v>
       </c>
       <c r="I3" s="1"/>
@@ -3257,28 +3268,28 @@
         <v>2</v>
       </c>
       <c r="B4" s="15" t="str">
-        <f>訊息格式說明!C6</f>
+        <f>訊息格式說明!C8</f>
         <v>版本</v>
       </c>
       <c r="C4" s="11">
-        <f>訊息格式說明!D6</f>
+        <f>訊息格式說明!D8</f>
         <v>4</v>
       </c>
       <c r="D4" s="11">
-        <f>訊息格式說明!E6</f>
+        <f>訊息格式說明!E8</f>
         <v>5</v>
       </c>
       <c r="E4" s="11">
-        <f>訊息格式說明!F6</f>
+        <f>訊息格式說明!F8</f>
         <v>2</v>
       </c>
       <c r="F4" s="11" t="str">
-        <f>訊息格式說明!G6</f>
+        <f>訊息格式說明!G8</f>
         <v>ushort</v>
       </c>
       <c r="G4" s="16"/>
       <c r="H4" s="17" t="str">
-        <f>訊息格式說明!I6</f>
+        <f>訊息格式說明!I8</f>
         <v>0x0100      (1.0)</v>
       </c>
       <c r="I4" s="1"/>
@@ -3288,28 +3299,28 @@
         <v>3</v>
       </c>
       <c r="B5" s="15" t="str">
-        <f>訊息格式說明!C7</f>
+        <f>訊息格式說明!C9</f>
         <v>保留欄位</v>
       </c>
       <c r="C5" s="11">
-        <f>訊息格式說明!D7</f>
+        <f>訊息格式說明!D9</f>
         <v>6</v>
       </c>
       <c r="D5" s="11">
-        <f>訊息格式說明!E7</f>
+        <f>訊息格式說明!E9</f>
         <v>7</v>
       </c>
       <c r="E5" s="11">
-        <f>訊息格式說明!F7</f>
+        <f>訊息格式說明!F9</f>
         <v>2</v>
       </c>
       <c r="F5" s="11" t="str">
-        <f>訊息格式說明!G7</f>
+        <f>訊息格式說明!G9</f>
         <v>ushort</v>
       </c>
       <c r="G5" s="18"/>
       <c r="H5" s="47">
-        <f>訊息格式說明!I7</f>
+        <f>訊息格式說明!I9</f>
         <v>0</v>
       </c>
       <c r="I5" s="1"/>
@@ -3319,23 +3330,23 @@
         <v>4</v>
       </c>
       <c r="B6" s="15" t="str">
-        <f>訊息格式說明!C8</f>
+        <f>訊息格式說明!C10</f>
         <v>訊息種類</v>
       </c>
       <c r="C6" s="11">
-        <f>訊息格式說明!D8</f>
+        <f>訊息格式說明!D10</f>
         <v>8</v>
       </c>
       <c r="D6" s="11">
-        <f>訊息格式說明!E8</f>
+        <f>訊息格式說明!E10</f>
         <v>8</v>
       </c>
       <c r="E6" s="11">
-        <f>訊息格式說明!F8</f>
+        <f>訊息格式說明!F10</f>
         <v>1</v>
       </c>
       <c r="F6" s="11" t="str">
-        <f>訊息格式說明!G8</f>
+        <f>訊息格式說明!G10</f>
         <v>byte</v>
       </c>
       <c r="G6" s="16"/>
@@ -3349,27 +3360,29 @@
         <v>5</v>
       </c>
       <c r="B7" s="15" t="str">
-        <f>訊息格式說明!C9</f>
+        <f>訊息格式說明!C11</f>
         <v>body長度</v>
       </c>
       <c r="C7" s="11">
-        <f>訊息格式說明!D9</f>
+        <f>訊息格式說明!D11</f>
         <v>9</v>
       </c>
       <c r="D7" s="11">
-        <f>訊息格式說明!E9</f>
+        <f>訊息格式說明!E11</f>
         <v>12</v>
       </c>
       <c r="E7" s="11">
-        <f>訊息格式說明!F9</f>
+        <f>訊息格式說明!F11</f>
         <v>4</v>
       </c>
       <c r="F7" s="11" t="str">
-        <f>訊息格式說明!G9</f>
+        <f>訊息格式說明!G11</f>
         <v>int</v>
       </c>
       <c r="G7" s="10"/>
-      <c r="H7" s="17"/>
+      <c r="H7" s="17">
+        <v>1</v>
+      </c>
       <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9" ht="57">
@@ -3380,7 +3393,7 @@
         <v>49</v>
       </c>
       <c r="C8" s="11">
-        <f>訊息格式說明!D10</f>
+        <f>訊息格式說明!D12</f>
         <v>13</v>
       </c>
       <c r="D8" s="11">
@@ -3404,28 +3417,28 @@
         <v>7</v>
       </c>
       <c r="B9" s="15" t="str">
-        <f>訊息格式說明!C11</f>
+        <f>訊息格式說明!C13</f>
         <v>CheckSum</v>
       </c>
       <c r="C9" s="11">
-        <f t="shared" ref="C8:C9" si="0">D8+1</f>
+        <f t="shared" ref="C9" si="0">D8+1</f>
         <v>14</v>
       </c>
       <c r="D9" s="11">
-        <f t="shared" ref="D8:D9" si="1">C9+E9-1</f>
+        <f t="shared" ref="D9" si="1">C9+E9-1</f>
         <v>14</v>
       </c>
       <c r="E9" s="11">
-        <f>訊息格式說明!F11</f>
+        <f>訊息格式說明!F13</f>
         <v>1</v>
       </c>
       <c r="F9" s="11" t="str">
-        <f>訊息格式說明!G11</f>
+        <f>訊息格式說明!G13</f>
         <v>byte</v>
       </c>
       <c r="G9" s="10"/>
       <c r="H9" s="17" t="str">
-        <f>訊息格式說明!I11</f>
+        <f>訊息格式說明!I13</f>
         <v>除起始字串及CheckSum外的欄位以XOR做加總</v>
       </c>
       <c r="I9" s="1"/>

</xml_diff>